<commit_message>
update to pitch freq effect size
</commit_message>
<xml_diff>
--- a/data for overview.xlsx
+++ b/data for overview.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ninai\Documents\Uni\3. semester\Experimental Methods III\A5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43ABA017-F2ED-497B-BF63-81F91EA051CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3605AB69-A053-4779-8FA7-3586D2FA1FFE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-4836" yWindow="3168" windowWidth="10008" windowHeight="10428" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MISURE" sheetId="2" r:id="rId1"/>
@@ -1234,7 +1234,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1283,6 +1283,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1297,7 +1303,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1496,6 +1502,19 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="8" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1782,10 +1801,10 @@
   <dimension ref="A1:FQ59"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <pane xSplit="6" ySplit="4" topLeftCell="BM5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="4" topLeftCell="BP44" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="BO21" sqref="BO21"/>
+      <selection pane="bottomRight" activeCell="E58" sqref="E58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.55" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2702,7 +2721,7 @@
       <c r="D4" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="21" t="s">
+      <c r="E4" s="74" t="s">
         <v>5</v>
       </c>
       <c r="F4" s="21">
@@ -3535,7 +3554,7 @@
       <c r="D10" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="28" t="s">
+      <c r="E10" s="73" t="s">
         <v>15</v>
       </c>
       <c r="F10" s="28">
@@ -3776,7 +3795,7 @@
       <c r="D12" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="E12" s="27" t="s">
+      <c r="E12" s="72" t="s">
         <v>17</v>
       </c>
       <c r="F12" s="28">
@@ -6735,7 +6754,7 @@
       <c r="D34" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="E34" s="2" t="s">
+      <c r="E34" s="71" t="s">
         <v>160</v>
       </c>
       <c r="F34" s="16">
@@ -7345,7 +7364,7 @@
       <c r="D37" s="18" t="s">
         <v>163</v>
       </c>
-      <c r="E37" s="2" t="s">
+      <c r="E37" s="71" t="s">
         <v>164</v>
       </c>
       <c r="F37" s="16">
@@ -7559,7 +7578,7 @@
       <c r="D38" s="18" t="s">
         <v>163</v>
       </c>
-      <c r="E38" s="2" t="s">
+      <c r="E38" s="71" t="s">
         <v>164</v>
       </c>
       <c r="F38" s="16">
@@ -9033,7 +9052,7 @@
       <c r="D47" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="E47" s="20" t="s">
+      <c r="E47" s="70" t="s">
         <v>254</v>
       </c>
       <c r="F47" s="20">
@@ -9597,7 +9616,7 @@
       <c r="D53" s="20" t="s">
         <v>272</v>
       </c>
-      <c r="E53" s="20" t="s">
+      <c r="E53" s="70" t="s">
         <v>273</v>
       </c>
       <c r="F53" s="20">
@@ -9785,7 +9804,7 @@
       <c r="D55" s="20" t="s">
         <v>319</v>
       </c>
-      <c r="E55" s="20" t="s">
+      <c r="E55" s="70" t="s">
         <v>317</v>
       </c>
       <c r="F55" s="20">

</xml_diff>